<commit_message>
Implemented BruteForce Traceback solution
</commit_message>
<xml_diff>
--- a/SudokuExcel.xlsx
+++ b/SudokuExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ctipub-my.sharepoint.com/personal/bogdan_voicu_stud_acs_upb_ro/Documents/Python/SudokuSolver/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_6A69C497014AD263E96D85924292E07542E5F9B2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C18A249E-154E-4F10-9BB8-196309966EBB}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="11_6A69C497017A5F4B0DCF9A924292E07542E5F9B2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90E7C706-8609-419F-A5E3-AEB19BEBB5C2}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -146,7 +146,7 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{38FB85B6-7DAD-4C7B-B43F-8FCA5B73D973}"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{08E82DA7-A6E7-4A99-8AAB-010427E10619}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -446,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,20 +462,36 @@
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
       <c r="F1" s="3"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="3"/>
+      <c r="G1" s="1">
+        <v>1</v>
+      </c>
+      <c r="H1" s="2">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
+      <c r="A2" s="4">
+        <v>8</v>
+      </c>
       <c r="C2" s="5"/>
       <c r="D2" s="4"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="4"/>
-      <c r="I2" s="5"/>
+      <c r="F2" s="5">
+        <v>7</v>
+      </c>
+      <c r="G2" s="4">
+        <v>4</v>
+      </c>
+      <c r="I2" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
       <c r="D3" s="6"/>
@@ -487,32 +503,49 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2">
+        <v>7</v>
+      </c>
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2">
+        <v>5</v>
+      </c>
       <c r="F4" s="3"/>
       <c r="G4" s="1"/>
       <c r="H4" s="2"/>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+      <c r="A5" s="4">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
       <c r="C5" s="5"/>
-      <c r="D5" s="4"/>
+      <c r="D5" s="4">
+        <v>8</v>
+      </c>
       <c r="F5" s="5"/>
-      <c r="G5" s="4">
-        <v>6</v>
-      </c>
-      <c r="I5" s="5"/>
+      <c r="G5" s="4"/>
+      <c r="I5" s="5">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
+      <c r="C6" s="8">
+        <v>8</v>
+      </c>
       <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="8"/>
+      <c r="E6" s="7">
+        <v>7</v>
+      </c>
+      <c r="F6" s="8">
+        <v>9</v>
+      </c>
       <c r="G6" s="6"/>
       <c r="H6" s="7"/>
       <c r="I6" s="8"/>
@@ -520,21 +553,38 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
+      <c r="C7" s="3">
+        <v>5</v>
+      </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2">
+        <v>9</v>
+      </c>
       <c r="F7" s="3"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2">
+        <v>3</v>
+      </c>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="4"/>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4">
+        <v>3</v>
+      </c>
       <c r="F8" s="5"/>
-      <c r="G8" s="4"/>
-      <c r="I8" s="5"/>
+      <c r="G8" s="4">
+        <v>5</v>
+      </c>
+      <c r="I8" s="5">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
@@ -542,14 +592,14 @@
       <c r="C9" s="8"/>
       <c r="D9" s="6"/>
       <c r="E9" s="7"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="6">
-        <v>6</v>
-      </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="8">
-        <v>6</v>
-      </c>
+      <c r="F9" s="8">
+        <v>4</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="7">
+        <v>8</v>
+      </c>
+      <c r="I9" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>